<commit_message>
add footer and 1 modal
</commit_message>
<xml_diff>
--- a/План.xlsx
+++ b/План.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>№</t>
   </si>
@@ -123,12 +123,6 @@
   </si>
   <si>
     <t>Готово</t>
-  </si>
-  <si>
-    <t>Всего: 14</t>
-  </si>
-  <si>
-    <t>Всего: 9</t>
   </si>
   <si>
     <t>Адаптивная версия</t>
@@ -563,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +603,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>32</v>
@@ -663,9 +657,7 @@
       <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="D5" s="6"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
@@ -696,9 +688,11 @@
       <c r="D7" s="1">
         <v>4</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -710,9 +704,11 @@
       <c r="D8" s="1">
         <v>2</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1">
+        <v>3.5</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -724,9 +720,11 @@
       <c r="D9" s="1">
         <v>1.5</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
       <c r="F9" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -738,9 +736,11 @@
       <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F10" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -752,9 +752,11 @@
       <c r="D11" s="1">
         <v>2</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <v>2.5</v>
+      </c>
       <c r="F11" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -766,9 +768,11 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>1.5</v>
+      </c>
       <c r="F12" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -781,9 +785,7 @@
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="D13" s="6"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
@@ -796,9 +798,11 @@
       <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1">
+        <v>2</v>
+      </c>
       <c r="F14" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -882,9 +886,11 @@
       <c r="D20" s="1">
         <v>1</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F20" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -892,7 +898,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1">
@@ -909,10 +915,14 @@
       <c r="C22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="1">
-        <v>32</v>
-      </c>
-      <c r="E22" s="1"/>
+      <c r="D22" s="6">
+        <f>SUM(D2:D21)</f>
+        <v>32</v>
+      </c>
+      <c r="E22" s="6">
+        <f>SUM(E2:E21)</f>
+        <v>31</v>
+      </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>